<commit_message>
added the points of event 2
</commit_message>
<xml_diff>
--- a/data/event1.xlsx
+++ b/data/event1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/e.saurov/PycharmProjects/sports_challenge/sports_challenge_dash/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D67F3A8-8010-A147-9487-77B43392EACA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE3D495-D6C6-D346-A9B3-D66C36C3214B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="26580" xr2:uid="{317BDA93-F79E-CD49-93E6-A149E0497E40}"/>
+    <workbookView xWindow="31000" yWindow="500" windowWidth="37800" windowHeight="26580" xr2:uid="{317BDA93-F79E-CD49-93E6-A149E0497E40}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Sum_7</t>
+  </si>
+  <si>
+    <t>Step-ups</t>
   </si>
 </sst>
 </file>
@@ -435,8 +438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D57FC62-670E-1B4D-86A9-E34F306EC0ED}">
   <dimension ref="A1:AC40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="AA3" sqref="AA3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="Z12" sqref="Z12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -665,7 +668,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="W3">
-        <f t="shared" ref="W3:W8" si="0">B3+C3+D3</f>
+        <f t="shared" ref="W3:W9" si="0">B3+C3+D3</f>
         <v>7.7</v>
       </c>
       <c r="X3">
@@ -673,7 +676,7 @@
         <v>7.3000000000000007</v>
       </c>
       <c r="Y3">
-        <f t="shared" ref="Y3:Y8" si="1">H3+I3+J3</f>
+        <f t="shared" ref="Y3:Y9" si="1">H3+I3+J3</f>
         <v>17.47</v>
       </c>
       <c r="Z3">
@@ -688,7 +691,7 @@
         <v>0</v>
       </c>
       <c r="AC3">
-        <f t="shared" ref="AC3:AC8" si="4">T3+U3+V3</f>
+        <f t="shared" ref="AC3:AC9" si="4">T3+U3+V3</f>
         <v>28.300000000000004</v>
       </c>
     </row>
@@ -764,7 +767,7 @@
         <v>13.68</v>
       </c>
       <c r="X4">
-        <f t="shared" ref="X4:X8" si="5">E4+F4+G4</f>
+        <f t="shared" ref="X4:X9" si="5">E4+F4+G4</f>
         <v>11</v>
       </c>
       <c r="Y4">
@@ -1152,11 +1155,11 @@
         <v>17.04</v>
       </c>
       <c r="Z8">
-        <f t="shared" si="2"/>
+        <f>K8+L8+M8</f>
         <v>4.2</v>
       </c>
       <c r="AA8">
-        <f t="shared" si="3"/>
+        <f>N8+O8+P8+Q8</f>
         <v>7.4799999999999995</v>
       </c>
       <c r="AB8">
@@ -1165,6 +1168,101 @@
       <c r="AC8">
         <f t="shared" si="4"/>
         <v>29.299999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>3.5</v>
+      </c>
+      <c r="C9">
+        <v>4.5</v>
+      </c>
+      <c r="D9">
+        <v>3.25</v>
+      </c>
+      <c r="E9">
+        <v>2.25</v>
+      </c>
+      <c r="F9">
+        <v>2.25</v>
+      </c>
+      <c r="G9">
+        <v>2.25</v>
+      </c>
+      <c r="H9">
+        <v>2.9</v>
+      </c>
+      <c r="I9">
+        <v>4</v>
+      </c>
+      <c r="J9">
+        <v>5.8</v>
+      </c>
+      <c r="K9">
+        <v>190</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>190</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>190</v>
+      </c>
+      <c r="T9">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="U9">
+        <v>2.5</v>
+      </c>
+      <c r="V9">
+        <v>2.6</v>
+      </c>
+      <c r="W9">
+        <f>190-(B9+C9+D9)</f>
+        <v>178.75</v>
+      </c>
+      <c r="X9">
+        <f>190-(E9+F9+G9)</f>
+        <v>183.25</v>
+      </c>
+      <c r="Y9">
+        <f>190-(H9+I9+J9)</f>
+        <v>177.3</v>
+      </c>
+      <c r="Z9">
+        <f>190-(K9+L9+M9)</f>
+        <v>0</v>
+      </c>
+      <c r="AA9">
+        <f>190-(N9+AO9+O9+P9+Q9)</f>
+        <v>0</v>
+      </c>
+      <c r="AB9">
+        <v>0</v>
+      </c>
+      <c r="AC9">
+        <f>190 -(T9+U9+V9)</f>
+        <v>182.6</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="23">

</xml_diff>

<commit_message>
error in excel corrected (wrong datetime)
</commit_message>
<xml_diff>
--- a/data/event1.xlsx
+++ b/data/event1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/e.saurov/PycharmProjects/sports_challenge/sports_challenge_dash/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE3D495-D6C6-D346-A9B3-D66C36C3214B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7EEFE7F-60AA-D04B-AE63-AFE1B6E62779}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31000" yWindow="500" windowWidth="37800" windowHeight="26580" xr2:uid="{317BDA93-F79E-CD49-93E6-A149E0497E40}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>Sum_7</t>
-  </si>
-  <si>
-    <t>Step-ups</t>
   </si>
 </sst>
 </file>
@@ -438,8 +435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D57FC62-670E-1B4D-86A9-E34F306EC0ED}">
   <dimension ref="A1:AC40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="Z12" sqref="Z12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -668,7 +665,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="W3">
-        <f t="shared" ref="W3:W9" si="0">B3+C3+D3</f>
+        <f t="shared" ref="W3:W8" si="0">B3+C3+D3</f>
         <v>7.7</v>
       </c>
       <c r="X3">
@@ -676,22 +673,22 @@
         <v>7.3000000000000007</v>
       </c>
       <c r="Y3">
-        <f t="shared" ref="Y3:Y9" si="1">H3+I3+J3</f>
+        <f t="shared" ref="Y3:Y8" si="1">H3+I3+J3</f>
         <v>17.47</v>
       </c>
       <c r="Z3">
-        <f t="shared" ref="Z3:Z8" si="2">K3+L3+M3</f>
+        <f t="shared" ref="Z3:Z7" si="2">K3+L3+M3</f>
         <v>10.4</v>
       </c>
       <c r="AA3">
-        <f t="shared" ref="AA3:AA8" si="3">N3+O3+P3+Q3</f>
+        <f t="shared" ref="AA3:AA7" si="3">N3+O3+P3+Q3</f>
         <v>4.9399999999999995</v>
       </c>
       <c r="AB3">
         <v>0</v>
       </c>
       <c r="AC3">
-        <f t="shared" ref="AC3:AC9" si="4">T3+U3+V3</f>
+        <f t="shared" ref="AC3:AC8" si="4">T3+U3+V3</f>
         <v>28.300000000000004</v>
       </c>
     </row>
@@ -767,7 +764,7 @@
         <v>13.68</v>
       </c>
       <c r="X4">
-        <f t="shared" ref="X4:X9" si="5">E4+F4+G4</f>
+        <f t="shared" ref="X4:X8" si="5">E4+F4+G4</f>
         <v>11</v>
       </c>
       <c r="Y4">
@@ -1171,8 +1168,8 @@
       </c>
     </row>
     <row r="9" spans="1:29">
-      <c r="A9" t="s">
-        <v>15</v>
+      <c r="A9" s="1">
+        <v>44576</v>
       </c>
       <c r="B9">
         <v>3.5</v>

</xml_diff>

<commit_message>
added results for the plank challange
</commit_message>
<xml_diff>
--- a/data/event1.xlsx
+++ b/data/event1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/e.saurov/PycharmProjects/sports_challenge/sports_challenge_dash/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B4E012-9C64-3C4A-91CC-50FA7DCD2EEA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6CCFDFE-7199-B440-81F8-FE7236F14A03}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31000" yWindow="500" windowWidth="37800" windowHeight="26580" xr2:uid="{317BDA93-F79E-CD49-93E6-A149E0497E40}"/>
   </bookViews>
@@ -436,10 +436,13 @@
   <dimension ref="A1:AC40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="AC11" sqref="AC11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="23" max="23" width="18.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:29">
       <c r="A1" t="s">
@@ -1260,6 +1263,102 @@
       <c r="AC9">
         <f>190 -(T9+U9+V9)</f>
         <v>182.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29">
+      <c r="A10" s="1">
+        <v>44583</v>
+      </c>
+      <c r="B10">
+        <v>3.93</v>
+      </c>
+      <c r="C10">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>3.25</v>
+      </c>
+      <c r="F10">
+        <v>1.83</v>
+      </c>
+      <c r="G10">
+        <v>3.75</v>
+      </c>
+      <c r="H10">
+        <v>3.08</v>
+      </c>
+      <c r="I10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J10">
+        <v>0.93</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>2.5</v>
+      </c>
+      <c r="U10">
+        <v>2</v>
+      </c>
+      <c r="V10">
+        <v>3.1</v>
+      </c>
+      <c r="W10">
+        <f>12*(B10+C10+D10)</f>
+        <v>145.56</v>
+      </c>
+      <c r="X10">
+        <f>12*(E10+F10+G10)</f>
+        <v>105.96000000000001</v>
+      </c>
+      <c r="Y10">
+        <f>12*(H10+I10+J10)</f>
+        <v>61.319999999999993</v>
+      </c>
+      <c r="Z10">
+        <f>12*(K10+L10+M10)</f>
+        <v>0</v>
+      </c>
+      <c r="AA10">
+        <f>12*(N10+O10+P10)</f>
+        <v>0</v>
+      </c>
+      <c r="AB10">
+        <f>12*(Q10+R10+S10)</f>
+        <v>0</v>
+      </c>
+      <c r="AC10">
+        <f>12*(T10+U10+V10)</f>
+        <v>91.199999999999989</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="23">

</xml_diff>

<commit_message>
updated the results after push-up event
</commit_message>
<xml_diff>
--- a/data/event1.xlsx
+++ b/data/event1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/e.saurov/PycharmProjects/sports_challenge/sports_challenge_dash/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6CCFDFE-7199-B440-81F8-FE7236F14A03}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEFFEF5E-7577-D04D-B823-5EF8A1622F35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31000" yWindow="500" windowWidth="37800" windowHeight="26580" xr2:uid="{317BDA93-F79E-CD49-93E6-A149E0497E40}"/>
   </bookViews>
@@ -436,7 +436,7 @@
   <dimension ref="A1:AC40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC11" sqref="AC11"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1359,6 +1359,116 @@
       <c r="AC10">
         <f>12*(T10+U10+V10)</f>
         <v>91.199999999999989</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29">
+      <c r="A11" s="1">
+        <v>44590</v>
+      </c>
+      <c r="B11">
+        <v>51</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>123</v>
+      </c>
+      <c r="F11">
+        <v>35</v>
+      </c>
+      <c r="G11">
+        <v>38</v>
+      </c>
+      <c r="H11">
+        <v>60</v>
+      </c>
+      <c r="I11">
+        <v>25</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>100</v>
+      </c>
+      <c r="U11">
+        <v>65</v>
+      </c>
+      <c r="V11">
+        <v>80</v>
+      </c>
+      <c r="W11">
+        <f>B11+C11+D11</f>
+        <v>51</v>
+      </c>
+      <c r="X11">
+        <f>E11+F11+G11</f>
+        <v>196</v>
+      </c>
+      <c r="Y11">
+        <f>H11+I11+J11</f>
+        <v>85</v>
+      </c>
+      <c r="Z11">
+        <f>K11+L11+M11</f>
+        <v>0</v>
+      </c>
+      <c r="AA11">
+        <f>N11+O11+P11</f>
+        <v>0</v>
+      </c>
+      <c r="AB11">
+        <f>Q11+R11+S11</f>
+        <v>0</v>
+      </c>
+      <c r="AC11">
+        <f>T11+U11+V11</f>
+        <v>245</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29">
+      <c r="A12" s="1">
+        <v>44611</v>
+      </c>
+      <c r="E12">
+        <v>200</v>
+      </c>
+      <c r="F12">
+        <v>350</v>
+      </c>
+      <c r="G12">
+        <v>455</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="23">

</xml_diff>

<commit_message>
updated the results of the final event (spartan challenge)
</commit_message>
<xml_diff>
--- a/data/event1.xlsx
+++ b/data/event1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/e.saurov/PycharmProjects/sports_challenge/sports_challenge_dash/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEFFEF5E-7577-D04D-B823-5EF8A1622F35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C7D213-4710-584D-BC4F-0644E369FC9D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31000" yWindow="500" windowWidth="37800" windowHeight="26580" xr2:uid="{317BDA93-F79E-CD49-93E6-A149E0497E40}"/>
   </bookViews>
@@ -436,7 +436,7 @@
   <dimension ref="A1:AC40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1461,6 +1461,15 @@
       <c r="A12" s="1">
         <v>44611</v>
       </c>
+      <c r="B12">
+        <v>375</v>
+      </c>
+      <c r="C12">
+        <v>355</v>
+      </c>
+      <c r="D12">
+        <v>380</v>
+      </c>
       <c r="E12">
         <v>200</v>
       </c>
@@ -1469,6 +1478,72 @@
       </c>
       <c r="G12">
         <v>455</v>
+      </c>
+      <c r="H12">
+        <v>262</v>
+      </c>
+      <c r="I12">
+        <v>339</v>
+      </c>
+      <c r="J12">
+        <v>339</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>214</v>
+      </c>
+      <c r="U12">
+        <v>204</v>
+      </c>
+      <c r="V12">
+        <v>234</v>
+      </c>
+      <c r="W12">
+        <v>100</v>
+      </c>
+      <c r="X12">
+        <v>150</v>
+      </c>
+      <c r="Y12">
+        <v>175</v>
+      </c>
+      <c r="Z12">
+        <v>0</v>
+      </c>
+      <c r="AA12">
+        <v>0</v>
+      </c>
+      <c r="AB12">
+        <v>0</v>
+      </c>
+      <c r="AC12">
+        <v>200</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="23">

</xml_diff>

<commit_message>
corrected a typo in results
</commit_message>
<xml_diff>
--- a/data/event1.xlsx
+++ b/data/event1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/e.saurov/PycharmProjects/sports_challenge/sports_challenge_dash/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C7D213-4710-584D-BC4F-0644E369FC9D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB1306A-844C-2D45-94B9-496C5CF4969D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31000" yWindow="500" windowWidth="37800" windowHeight="26580" xr2:uid="{317BDA93-F79E-CD49-93E6-A149E0497E40}"/>
   </bookViews>
@@ -435,8 +435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D57FC62-670E-1B4D-86A9-E34F306EC0ED}">
   <dimension ref="A1:AC40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1483,10 +1483,10 @@
         <v>262</v>
       </c>
       <c r="I12">
-        <v>339</v>
+        <v>375</v>
       </c>
       <c r="J12">
-        <v>339</v>
+        <v>375</v>
       </c>
       <c r="K12">
         <v>0</v>

</xml_diff>